<commit_message>
feat: add CLI chat demo, improve path handling, and update README with setup instructions
</commit_message>
<xml_diff>
--- a/excel_ocr/output/financial_summary.xlsx
+++ b/excel_ocr/output/financial_summary.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t xml:space="preserve"> Indicator</t>
   </si>
   <si>
-    <t>Current Year (2024)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous Year (2023) </t>
+    <t>2024 (Previous Year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 (Current Year) </t>
   </si>
   <si>
     <t xml:space="preserve"> Cash and Cash Equivalents</t>
@@ -31,100 +31,61 @@
     <t xml:space="preserve"> Accounts Receivable</t>
   </si>
   <si>
-    <t xml:space="preserve"> Property, Plant and Equipment</t>
+    <t xml:space="preserve"> Total Current Assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Non-current Assets</t>
   </si>
   <si>
     <t xml:space="preserve"> Total Assets</t>
   </si>
   <si>
-    <t xml:space="preserve"> Accounts Payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Retained Earnings</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Total Equity &amp; Liabilities</t>
+    <t xml:space="preserve"> Total Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Liabilities and Equity</t>
   </si>
   <si>
     <t xml:space="preserve"> Revenue</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cost of Goods Sold (COGS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> General and Administrative Expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Profit Before Tax</t>
+    <t xml:space="preserve"> Cost of Goods Sold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gross Profit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Operating Profit</t>
   </si>
   <si>
     <t xml:space="preserve"> Net Profit</t>
   </si>
   <si>
-    <t>1,000</t>
-  </si>
-  <si>
-    <t>11,987,605.97</t>
-  </si>
-  <si>
-    <t>3,489,523.92</t>
-  </si>
-  <si>
-    <t>14,355,193.96</t>
-  </si>
-  <si>
-    <t>-12,443,892.15</t>
-  </si>
-  <si>
-    <t>-2,444,853.69</t>
-  </si>
-  <si>
-    <t>-14,888,745.84</t>
-  </si>
-  <si>
-    <t>-1,276,151.85</t>
-  </si>
-  <si>
-    <t>-367,148.33</t>
-  </si>
-  <si>
-    <t>937,434.64</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,000                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,711,454.12        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,494,523.92         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,424,369.47        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-10,979,515.78       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,741,596.38        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,721,112.16        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,727,145.61        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-428,513.69          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,105,786.47         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A                  </t>
+    <t xml:space="preserve"> Net Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cash Flow from Operating Activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Net Change in Cash</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7000 - 1000          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5000 - 3000 - 1500) </t>
   </si>
 </sst>
 </file>
@@ -482,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,10 +465,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -515,10 +476,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -526,10 +487,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -537,10 +498,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -551,7 +512,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -559,10 +520,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -570,32 +531,32 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -603,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -614,10 +575,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -625,10 +586,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -636,10 +597,65 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>